<commit_message>
Excel mis à jour
</commit_message>
<xml_diff>
--- a/res/SyntheseRH.xlsx
+++ b/res/SyntheseRH.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ndugue\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IUTtravail\cours\excel\Excel20192020\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D872666-1ADB-4036-A6D4-1BCEC331081E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="7455" tabRatio="500"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="3" r:id="rId1"/>
@@ -23,8 +24,7 @@
     <definedName name="solver_val" localSheetId="0">0</definedName>
     <definedName name="solver_ver" localSheetId="0">3</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-40C];[Red]\-#,##0.00\ [$€-40C]"/>
   </numFmts>
@@ -672,27 +672,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="5" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="11" width="10.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="7" max="11" width="10.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" customWidth="1"/>
     <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="1025" width="10.7109375" customWidth="1"/>
+    <col min="14" max="1025" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -732,7 +732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -766,7 +766,7 @@
         <v>4734</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -800,7 +800,7 @@
         <v>8550</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -834,7 +834,7 @@
         <v>3367</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>23</v>
       </c>
@@ -868,7 +868,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1988</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>29</v>
       </c>
@@ -932,7 +932,7 @@
         <v>2511</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
@@ -961,7 +961,7 @@
         <v>4998</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
@@ -990,7 +990,7 @@
         <v>2997</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
@@ -1019,7 +1019,7 @@
         <v>3031</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>3527</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
         <v>40</v>
       </c>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="J13" s="2"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D14" s="2" t="s">
         <v>41</v>
       </c>
@@ -1099,7 +1099,7 @@
       </c>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
         <v>42</v>
       </c>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="J15" s="2"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="J16" s="2"/>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="J17" s="2"/>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
@@ -1167,7 +1167,7 @@
       </c>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D19" s="2" t="s">
         <v>46</v>
       </c>
@@ -1184,7 +1184,7 @@
       </c>
       <c r="J19" s="2"/>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="J20" s="2"/>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D21" s="2" t="s">
         <v>48</v>
       </c>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="J21" s="2"/>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D22" s="2" t="s">
         <v>49</v>
       </c>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D23" s="2" t="s">
         <v>50</v>
       </c>
@@ -1252,7 +1252,7 @@
       </c>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D24" s="2" t="s">
         <v>51</v>
       </c>
@@ -1269,7 +1269,7 @@
       </c>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D25" s="2" t="s">
         <v>52</v>
       </c>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D26" s="2" t="s">
         <v>53</v>
       </c>
@@ -1303,7 +1303,7 @@
       </c>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D27" s="2" t="s">
         <v>54</v>
       </c>
@@ -1320,7 +1320,7 @@
       </c>
       <c r="J27" s="2"/>
     </row>
-    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D28" s="2" t="s">
         <v>55</v>
       </c>
@@ -1337,7 +1337,7 @@
       </c>
       <c r="J28" s="2"/>
     </row>
-    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="J29" s="2"/>
     </row>
-    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D30" s="2" t="s">
         <v>57</v>
       </c>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="J30" s="2"/>
     </row>
-    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D31" s="2" t="s">
         <v>58</v>
       </c>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="J31" s="2"/>
     </row>
-    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D32" s="2" t="s">
         <v>59</v>
       </c>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="J32" s="2"/>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D33" s="2" t="s">
         <v>60</v>
       </c>
@@ -1422,7 +1422,7 @@
       </c>
       <c r="J33" s="2"/>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D34" s="2" t="s">
         <v>61</v>
       </c>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="J34" s="2"/>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D35" s="2" t="s">
         <v>62</v>
       </c>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="J35" s="2"/>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D36" s="2" t="s">
         <v>63</v>
       </c>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="J36" s="2"/>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D37" s="2" t="s">
         <v>64</v>
       </c>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D38" s="2" t="s">
         <v>65</v>
       </c>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D39" s="2" t="s">
         <v>66</v>
       </c>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D40" s="2" t="s">
         <v>67</v>
       </c>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D41" s="2" t="s">
         <v>68</v>
       </c>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D42" s="2" t="s">
         <v>69</v>
       </c>

</xml_diff>